<commit_message>
NCC with feature data error fix on the eu find distance
</commit_message>
<xml_diff>
--- a/Experiment result/Histogram vs Feature Data/All Result.xlsx
+++ b/Experiment result/Histogram vs Feature Data/All Result.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20350"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20351"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87E870EB-5B49-47C9-BCF5-47BE8E3DEEDF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A42F27D2-37FE-49BE-9ADC-4393121D2321}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>NCC with Feature</t>
   </si>
@@ -38,18 +38,6 @@
   </si>
   <si>
     <t>Single Model with histogram</t>
-  </si>
-  <si>
-    <t>Sum</t>
-  </si>
-  <si>
-    <t>Average</t>
-  </si>
-  <si>
-    <t>Running Total</t>
-  </si>
-  <si>
-    <t>Count</t>
   </si>
   <si>
     <t>2+3</t>
@@ -248,22 +236,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.42142049145346755</c:v>
+                  <c:v>0.18909089850313116</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.41786959709421612</c:v>
+                  <c:v>0.1883158691412665</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.41577080992535143</c:v>
+                  <c:v>0.18950428968160471</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.41207228361829218</c:v>
+                  <c:v>0.18206111442472653</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.41956836062968705</c:v>
+                  <c:v>0.18689628297044972</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.42238913088258601</c:v>
+                  <c:v>0.18708011148677436</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1468,16 +1456,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>104774</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>23811</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>166686</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>266699</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>159066</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>111441</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1771,7 +1759,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1785,23 +1773,23 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1">
-        <v>0.42142049145346755</v>
-      </c>
-      <c r="C1" s="1">
-        <v>0.41786959709421612</v>
-      </c>
-      <c r="D1" s="1">
-        <v>0.41577080992535143</v>
-      </c>
-      <c r="E1" s="1">
-        <v>0.41207228361829218</v>
-      </c>
-      <c r="F1" s="1">
-        <v>0.41956836062968705</v>
-      </c>
-      <c r="G1" s="1">
-        <v>0.42238913088258601</v>
+      <c r="B1">
+        <v>0.18909089850313116</v>
+      </c>
+      <c r="C1">
+        <v>0.1883158691412665</v>
+      </c>
+      <c r="D1">
+        <v>0.18950428968160471</v>
+      </c>
+      <c r="E1">
+        <v>0.18206111442472653</v>
+      </c>
+      <c r="F1">
+        <v>0.18689628297044972</v>
+      </c>
+      <c r="G1">
+        <v>0.18708011148677436</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1921,7 +1909,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C7" s="1">
         <v>4</v>

</xml_diff>

<commit_message>
Add new code for normalizing all data (100 user) in 6 period
</commit_message>
<xml_diff>
--- a/Experiment result/Histogram vs Feature Data/All Result.xlsx
+++ b/Experiment result/Histogram vs Feature Data/All Result.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20351"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A42F27D2-37FE-49BE-9ADC-4393121D2321}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8736AF0B-A81D-4CF9-AA5A-CFAB9B888F5A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>NCC with Feature</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>NCC with histogram</t>
   </si>
@@ -41,6 +38,12 @@
   </si>
   <si>
     <t>2+3</t>
+  </si>
+  <si>
+    <t>NCC with Feature normalized data per period</t>
+  </si>
+  <si>
+    <t>NCC with Feature normalized all data</t>
   </si>
 </sst>
 </file>
@@ -182,11 +185,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$1</c:f>
+              <c:f>Sheet1!$A$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>NCC with Feature</c:v>
+                  <c:v>NCC with Feature normalized data per period</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -205,7 +208,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$7:$G$7</c:f>
+              <c:f>Sheet1!$B$8:$G$8</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -231,27 +234,27 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$1:$G$1</c:f>
+              <c:f>Sheet1!$B$2:$G$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.18909089850313116</c:v>
+                  <c:v>0.1943969959451371</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.1883158691412665</c:v>
+                  <c:v>0.19309247794222512</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.18950428968160471</c:v>
+                  <c:v>0.19343414031686831</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.18206111442472653</c:v>
+                  <c:v>0.18530010899272892</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.18689628297044972</c:v>
+                  <c:v>0.19101750938172032</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.18708011148677436</c:v>
+                  <c:v>0.19204771504129037</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -268,7 +271,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$2</c:f>
+              <c:f>Sheet1!$A$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -291,7 +294,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$7:$G$7</c:f>
+              <c:f>Sheet1!$B$8:$G$8</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -317,7 +320,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$G$2</c:f>
+              <c:f>Sheet1!$B$3:$G$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -354,7 +357,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$3</c:f>
+              <c:f>Sheet1!$A$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -377,7 +380,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$7:$G$7</c:f>
+              <c:f>Sheet1!$B$8:$G$8</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -403,7 +406,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$G$3</c:f>
+              <c:f>Sheet1!$B$4:$G$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -440,7 +443,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$4</c:f>
+              <c:f>Sheet1!$A$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -463,7 +466,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$7:$G$7</c:f>
+              <c:f>Sheet1!$B$8:$G$8</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -489,7 +492,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$4:$G$4</c:f>
+              <c:f>Sheet1!$B$5:$G$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -526,7 +529,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$5</c:f>
+              <c:f>Sheet1!$A$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -549,7 +552,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$7:$G$7</c:f>
+              <c:f>Sheet1!$B$8:$G$8</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -575,7 +578,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$5:$G$5</c:f>
+              <c:f>Sheet1!$B$6:$G$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -612,7 +615,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$6</c:f>
+              <c:f>Sheet1!$A$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -635,7 +638,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$7:$G$7</c:f>
+              <c:f>Sheet1!$B$8:$G$8</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -661,7 +664,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$6:$G$6</c:f>
+              <c:f>Sheet1!$B$7:$G$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -690,6 +693,68 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000005-8771-4447-A535-59A6EE4ED78D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>NCC with Feature normalized all data</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$1:$G$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.19162794729540647</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.18857952947862608</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.19208493755102754</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.18039645639795629</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.19096668589114685</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.18956224341147718</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-9051-4415-90F3-FFD58CAE7B8A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1458,14 +1523,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>166686</xdr:rowOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>14286</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>111441</xdr:rowOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>149541</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1756,174 +1821,198 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.140625" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" style="1" customWidth="1"/>
-    <col min="3" max="7" width="9.140625" style="1"/>
+    <col min="1" max="1" width="44.28515625" customWidth="1"/>
+    <col min="2" max="2" width="14" style="1" customWidth="1"/>
+    <col min="3" max="6" width="13.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1">
-        <v>0.18909089850313116</v>
-      </c>
-      <c r="C1">
-        <v>0.1883158691412665</v>
-      </c>
-      <c r="D1">
-        <v>0.18950428968160471</v>
-      </c>
-      <c r="E1">
-        <v>0.18206111442472653</v>
-      </c>
-      <c r="F1">
-        <v>0.18689628297044972</v>
-      </c>
-      <c r="G1">
-        <v>0.18708011148677436</v>
+        <v>7</v>
+      </c>
+      <c r="B1" s="1">
+        <v>0.19162794729540647</v>
+      </c>
+      <c r="C1" s="1">
+        <v>0.18857952947862608</v>
+      </c>
+      <c r="D1" s="1">
+        <v>0.19208493755102754</v>
+      </c>
+      <c r="E1" s="1">
+        <v>0.18039645639795629</v>
+      </c>
+      <c r="F1" s="1">
+        <v>0.19096668589114685</v>
+      </c>
+      <c r="G1" s="1">
+        <v>0.18956224341147718</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1">
-        <v>2.6907665109083954E-2</v>
+        <v>0.1943969959451371</v>
       </c>
       <c r="C2" s="1">
-        <v>2.7612677667900307E-2</v>
+        <v>0.19309247794222512</v>
       </c>
       <c r="D2" s="1">
-        <v>2.7146835832719565E-2</v>
+        <v>0.19343414031686831</v>
       </c>
       <c r="E2" s="1">
-        <v>2.7154750628444843E-2</v>
+        <v>0.18530010899272892</v>
       </c>
       <c r="F2" s="1">
-        <v>2.9197552407460258E-2</v>
+        <v>0.19101750938172032</v>
       </c>
       <c r="G2" s="1">
-        <v>2.7955516355071791E-2</v>
+        <v>0.19204771504129037</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B3" s="1">
-        <v>9.7086118676726951E-2</v>
+        <v>2.6907665109083954E-2</v>
       </c>
       <c r="C3" s="1">
-        <v>8.9843163588435818E-2</v>
+        <v>2.7612677667900307E-2</v>
       </c>
       <c r="D3" s="1">
-        <v>8.9094256838943314E-2</v>
+        <v>2.7146835832719565E-2</v>
       </c>
       <c r="E3" s="1">
-        <v>8.9298878977829316E-2</v>
+        <v>2.7154750628444843E-2</v>
       </c>
       <c r="F3" s="1">
-        <v>9.0172300910407011E-2</v>
+        <v>2.9197552407460258E-2</v>
       </c>
       <c r="G3" s="1">
-        <v>8.4278646259511175E-2</v>
+        <v>2.7955516355071791E-2</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B4" s="1">
-        <v>2.6055865971738066E-2</v>
+        <v>9.7086118676726951E-2</v>
       </c>
       <c r="C4" s="1">
-        <v>2.1233263904043134E-2</v>
+        <v>8.9843163588435818E-2</v>
       </c>
       <c r="D4" s="1">
-        <v>2.4886672316570012E-2</v>
+        <v>8.9094256838943314E-2</v>
       </c>
       <c r="E4" s="1">
-        <v>2.3017383133662212E-2</v>
+        <v>8.9298878977829316E-2</v>
       </c>
       <c r="F4" s="1">
-        <v>2.2846725260503225E-2</v>
+        <v>9.0172300910407011E-2</v>
       </c>
       <c r="G4" s="1">
-        <v>2.0546996721796374E-2</v>
+        <v>8.4278646259511175E-2</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B5" s="1">
-        <v>9.7086118676726951E-2</v>
+        <v>2.6055865971738066E-2</v>
       </c>
       <c r="C5" s="1">
-        <v>0.15419419485172386</v>
+        <v>2.1233263904043134E-2</v>
       </c>
       <c r="D5" s="1">
-        <v>0.15331153775641479</v>
+        <v>2.4886672316570012E-2</v>
       </c>
       <c r="E5" s="1">
-        <v>0.15649588812551726</v>
+        <v>2.3017383133662212E-2</v>
       </c>
       <c r="F5" s="1">
-        <v>0.16602972448750986</v>
+        <v>2.2846725260503225E-2</v>
       </c>
       <c r="G5" s="1">
-        <v>0.17326214624472261</v>
+        <v>2.0546996721796374E-2</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B6" s="1">
-        <v>2.6055865971738066E-2</v>
+        <v>9.7086118676726951E-2</v>
       </c>
       <c r="C6" s="1">
-        <v>7.3711973203230932E-2</v>
+        <v>0.15419419485172386</v>
       </c>
       <c r="D6" s="1">
-        <v>8.2858705628974114E-2</v>
+        <v>0.15331153775641479</v>
       </c>
       <c r="E6" s="1">
-        <v>8.668301439495614E-2</v>
+        <v>0.15649588812551726</v>
       </c>
       <c r="F6" s="1">
-        <v>9.6543995614224193E-2</v>
+        <v>0.16602972448750986</v>
       </c>
       <c r="G6" s="1">
-        <v>8.8661260487628707E-2</v>
+        <v>0.17326214624472261</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="1" t="s">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="1">
+        <v>2.6055865971738066E-2</v>
+      </c>
+      <c r="C7" s="1">
+        <v>7.3711973203230932E-2</v>
+      </c>
+      <c r="D7" s="1">
+        <v>8.2858705628974114E-2</v>
+      </c>
+      <c r="E7" s="1">
+        <v>8.668301439495614E-2</v>
+      </c>
+      <c r="F7" s="1">
+        <v>9.6543995614224193E-2</v>
+      </c>
+      <c r="G7" s="1">
+        <v>8.8661260487628707E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="1">
+        <v>4</v>
+      </c>
+      <c r="D8" s="1">
+        <v>5</v>
+      </c>
+      <c r="E8" s="1">
         <v>6</v>
       </c>
-      <c r="C7" s="1">
-        <v>4</v>
-      </c>
-      <c r="D7" s="1">
-        <v>5</v>
-      </c>
-      <c r="E7" s="1">
-        <v>6</v>
-      </c>
-      <c r="F7" s="1">
+      <c r="F8" s="1">
         <v>7</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G8" s="1">
         <v>8</v>
       </c>
     </row>

</xml_diff>